<commit_message>
Updated Test Case for Customer
</commit_message>
<xml_diff>
--- a/documentation/quality/Test Documents/02-TC-Customers.xlsx
+++ b/documentation/quality/Test Documents/02-TC-Customers.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HostedRBI\apc-softdev-it111-06\documentation\quality\Test Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="2940" windowWidth="19440" windowHeight="8400"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="265">
   <si>
     <t>Tester:</t>
   </si>
@@ -1515,8 +1520,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1937,6 +1942,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1984,7 +1992,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2016,9 +2024,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2050,6 +2059,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2225,14 +2235,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
@@ -2242,7 +2252,7 @@
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>152</v>
       </c>
@@ -2253,7 +2263,7 @@
       <c r="F1" s="61"/>
       <c r="G1" s="62"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
@@ -2279,7 +2289,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
         <v>1</v>
       </c>
@@ -2290,27 +2300,27 @@
       <c r="F3" s="58"/>
       <c r="G3" s="59"/>
       <c r="I3" s="63">
-        <f>AVERAGE(Sheet2!B17/85)</f>
+        <f>AVERAGE(Sheet2!B18/85)</f>
         <v>0</v>
       </c>
       <c r="J3" s="63">
-        <f>AVERAGE(Sheet2!C17/85)</f>
+        <f>AVERAGE(Sheet2!C18/85)</f>
         <v>0</v>
       </c>
       <c r="K3" s="63">
-        <f>AVERAGE(Sheet2!D17/85)</f>
-        <v>0.87058823529411766</v>
+        <f>AVERAGE(Sheet2!D18/82)</f>
+        <v>1</v>
       </c>
       <c r="L3" s="63">
-        <f>AVERAGE(Sheet2!E17/85)</f>
+        <f>AVERAGE(Sheet2!E18/85)</f>
         <v>0</v>
       </c>
       <c r="M3" s="63">
         <f>SUM(I3:L4)</f>
-        <v>0.87058823529411766</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="54" t="s">
         <v>120</v>
       </c>
@@ -2326,7 +2336,7 @@
       <c r="L4" s="63"/>
       <c r="M4" s="63"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>2</v>
       </c>
@@ -2339,7 +2349,7 @@
       <c r="F5" s="48"/>
       <c r="G5" s="49"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>2</v>
       </c>
@@ -2362,7 +2372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="120.75" customHeight="1" thickBot="1">
+    <row r="7" spans="1:15" ht="120.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>37</v>
       </c>
@@ -2388,7 +2398,7 @@
       <c r="N7" s="52"/>
       <c r="O7" s="53"/>
     </row>
-    <row r="8" spans="1:15" ht="150">
+    <row r="8" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>39</v>
       </c>
@@ -2406,7 +2416,7 @@
       <c r="G8" s="22"/>
       <c r="I8" s="50"/>
     </row>
-    <row r="9" spans="1:15" ht="165">
+    <row r="9" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>40</v>
       </c>
@@ -2423,7 +2433,7 @@
       </c>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:15" ht="195">
+    <row r="10" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>41</v>
       </c>
@@ -2440,7 +2450,7 @@
       </c>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="1:15" ht="135">
+    <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>45</v>
       </c>
@@ -2457,7 +2467,7 @@
       </c>
       <c r="G11" s="22"/>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1">
+    <row r="12" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>2.1</v>
       </c>
@@ -2470,7 +2480,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="32"/>
     </row>
-    <row r="13" spans="1:15" ht="60">
+    <row r="13" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>46</v>
       </c>
@@ -2487,7 +2497,7 @@
       </c>
       <c r="G13" s="22"/>
     </row>
-    <row r="14" spans="1:15" ht="60">
+    <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>47</v>
       </c>
@@ -2504,7 +2514,7 @@
       </c>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="1:15" ht="45">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>48</v>
       </c>
@@ -2521,7 +2531,7 @@
       </c>
       <c r="G15" s="22"/>
     </row>
-    <row r="16" spans="1:15" ht="30">
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>2.2000000000000002</v>
       </c>
@@ -2534,7 +2544,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="36"/>
     </row>
-    <row r="17" spans="1:7" ht="75">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>132</v>
       </c>
@@ -2551,7 +2561,7 @@
       </c>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="1:7" ht="150">
+    <row r="18" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>52</v>
       </c>
@@ -2568,7 +2578,7 @@
       </c>
       <c r="G18" s="22"/>
     </row>
-    <row r="19" spans="1:7" ht="180">
+    <row r="19" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>53</v>
       </c>
@@ -2585,7 +2595,7 @@
       </c>
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="1:7" ht="150">
+    <row r="20" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>133</v>
       </c>
@@ -2602,7 +2612,7 @@
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="1:7" ht="60">
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>54</v>
       </c>
@@ -2619,7 +2629,7 @@
       </c>
       <c r="G21" s="22"/>
     </row>
-    <row r="22" spans="1:7" ht="135">
+    <row r="22" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>55</v>
       </c>
@@ -2636,7 +2646,7 @@
       </c>
       <c r="G22" s="22"/>
     </row>
-    <row r="23" spans="1:7" ht="120">
+    <row r="23" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>56</v>
       </c>
@@ -2653,7 +2663,7 @@
       </c>
       <c r="G23" s="22"/>
     </row>
-    <row r="24" spans="1:7" ht="120">
+    <row r="24" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>57</v>
       </c>
@@ -2670,7 +2680,7 @@
       </c>
       <c r="G24" s="22"/>
     </row>
-    <row r="25" spans="1:7" ht="120">
+    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>58</v>
       </c>
@@ -2687,7 +2697,7 @@
       </c>
       <c r="G25" s="22"/>
     </row>
-    <row r="26" spans="1:7" ht="165">
+    <row r="26" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>59</v>
       </c>
@@ -2704,7 +2714,7 @@
       </c>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:7" ht="120">
+    <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>60</v>
       </c>
@@ -2721,7 +2731,7 @@
       </c>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="1:7" ht="135">
+    <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>61</v>
       </c>
@@ -2738,7 +2748,7 @@
       </c>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:7" ht="135">
+    <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>62</v>
       </c>
@@ -2755,7 +2765,7 @@
       </c>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:7" ht="165">
+    <row r="30" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>63</v>
       </c>
@@ -2772,7 +2782,7 @@
       </c>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:7" ht="30">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>2.2999999999999998</v>
       </c>
@@ -2785,7 +2795,7 @@
       <c r="F31" s="8"/>
       <c r="G31" s="36"/>
     </row>
-    <row r="32" spans="1:7" ht="120">
+    <row r="32" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>80</v>
       </c>
@@ -2802,7 +2812,7 @@
       </c>
       <c r="G32" s="22"/>
     </row>
-    <row r="33" spans="1:7" ht="60">
+    <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>81</v>
       </c>
@@ -2819,7 +2829,7 @@
       </c>
       <c r="G33" s="22"/>
     </row>
-    <row r="34" spans="1:7" ht="135">
+    <row r="34" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>82</v>
       </c>
@@ -2836,7 +2846,7 @@
       </c>
       <c r="G34" s="22"/>
     </row>
-    <row r="35" spans="1:7" ht="135">
+    <row r="35" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>83</v>
       </c>
@@ -2853,7 +2863,7 @@
       </c>
       <c r="G35" s="22"/>
     </row>
-    <row r="36" spans="1:7" ht="120">
+    <row r="36" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>84</v>
       </c>
@@ -2870,7 +2880,7 @@
       </c>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" spans="1:7" ht="120">
+    <row r="37" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>85</v>
       </c>
@@ -2887,7 +2897,7 @@
       </c>
       <c r="G37" s="22"/>
     </row>
-    <row r="38" spans="1:7" ht="120">
+    <row r="38" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>86</v>
       </c>
@@ -2904,7 +2914,7 @@
       </c>
       <c r="G38" s="22"/>
     </row>
-    <row r="39" spans="1:7" ht="45">
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>87</v>
       </c>
@@ -2921,7 +2931,7 @@
       </c>
       <c r="G39" s="22"/>
     </row>
-    <row r="40" spans="1:7" ht="120">
+    <row r="40" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>88</v>
       </c>
@@ -2938,7 +2948,7 @@
       </c>
       <c r="G40" s="22"/>
     </row>
-    <row r="41" spans="1:7" ht="120">
+    <row r="41" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>89</v>
       </c>
@@ -2955,7 +2965,7 @@
       </c>
       <c r="G41" s="22"/>
     </row>
-    <row r="42" spans="1:7" ht="60">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>90</v>
       </c>
@@ -2972,7 +2982,7 @@
       </c>
       <c r="G42" s="22"/>
     </row>
-    <row r="43" spans="1:7" ht="45">
+    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>91</v>
       </c>
@@ -2989,7 +2999,7 @@
       </c>
       <c r="G43" s="22"/>
     </row>
-    <row r="44" spans="1:7" ht="45">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>179</v>
       </c>
@@ -3002,7 +3012,7 @@
       <c r="F44" s="8"/>
       <c r="G44" s="36"/>
     </row>
-    <row r="45" spans="1:7" ht="75">
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
         <v>186</v>
       </c>
@@ -3019,7 +3029,7 @@
       </c>
       <c r="G45" s="22"/>
     </row>
-    <row r="46" spans="1:7" ht="75">
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
         <v>187</v>
       </c>
@@ -3036,7 +3046,7 @@
       </c>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="1:7" ht="75">
+    <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="23" t="s">
         <v>188</v>
       </c>
@@ -3053,7 +3063,7 @@
       </c>
       <c r="G47" s="22"/>
     </row>
-    <row r="48" spans="1:7" ht="60">
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
         <v>189</v>
       </c>
@@ -3070,7 +3080,7 @@
       </c>
       <c r="G48" s="22"/>
     </row>
-    <row r="49" spans="1:7" ht="60">
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>190</v>
       </c>
@@ -3087,7 +3097,7 @@
       </c>
       <c r="G49" s="22"/>
     </row>
-    <row r="50" spans="1:7" ht="60">
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>191</v>
       </c>
@@ -3104,7 +3114,7 @@
       </c>
       <c r="G50" s="22"/>
     </row>
-    <row r="51" spans="1:7" ht="30">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>192</v>
       </c>
@@ -3121,7 +3131,7 @@
       </c>
       <c r="G51" s="22"/>
     </row>
-    <row r="52" spans="1:7" ht="45">
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
         <v>193</v>
       </c>
@@ -3138,7 +3148,7 @@
       </c>
       <c r="G52" s="22"/>
     </row>
-    <row r="53" spans="1:7" ht="30">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="28">
         <v>2.4</v>
       </c>
@@ -3151,7 +3161,7 @@
       <c r="F53" s="10"/>
       <c r="G53" s="29"/>
     </row>
-    <row r="54" spans="1:7" ht="90">
+    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>134</v>
       </c>
@@ -3168,7 +3178,7 @@
       </c>
       <c r="G54" s="22"/>
     </row>
-    <row r="55" spans="1:7" ht="75">
+    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>94</v>
       </c>
@@ -3185,7 +3195,7 @@
       </c>
       <c r="G55" s="22"/>
     </row>
-    <row r="56" spans="1:7" ht="90">
+    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>95</v>
       </c>
@@ -3202,7 +3212,7 @@
       </c>
       <c r="G56" s="22"/>
     </row>
-    <row r="57" spans="1:7" ht="75">
+    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>96</v>
       </c>
@@ -3219,7 +3229,7 @@
       </c>
       <c r="G57" s="22"/>
     </row>
-    <row r="58" spans="1:7" ht="75">
+    <row r="58" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>97</v>
       </c>
@@ -3236,7 +3246,7 @@
       </c>
       <c r="G58" s="22"/>
     </row>
-    <row r="59" spans="1:7" ht="75">
+    <row r="59" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>98</v>
       </c>
@@ -3253,7 +3263,7 @@
       </c>
       <c r="G59" s="22"/>
     </row>
-    <row r="60" spans="1:7" ht="150">
+    <row r="60" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>99</v>
       </c>
@@ -3270,7 +3280,7 @@
       </c>
       <c r="G60" s="22"/>
     </row>
-    <row r="61" spans="1:7" ht="30">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="28">
         <v>2.5</v>
       </c>
@@ -3283,7 +3293,7 @@
       <c r="F61" s="10"/>
       <c r="G61" s="29"/>
     </row>
-    <row r="62" spans="1:7" ht="75">
+    <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
         <v>115</v>
       </c>
@@ -3300,7 +3310,7 @@
       </c>
       <c r="G62" s="22"/>
     </row>
-    <row r="63" spans="1:7" ht="60">
+    <row r="63" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
         <v>116</v>
       </c>
@@ -3317,7 +3327,7 @@
       </c>
       <c r="G63" s="22"/>
     </row>
-    <row r="64" spans="1:7" ht="75">
+    <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>117</v>
       </c>
@@ -3334,7 +3344,7 @@
       </c>
       <c r="G64" s="22"/>
     </row>
-    <row r="65" spans="1:7" ht="150">
+    <row r="65" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>118</v>
       </c>
@@ -3351,7 +3361,7 @@
       </c>
       <c r="G65" s="22"/>
     </row>
-    <row r="66" spans="1:7" ht="60">
+    <row r="66" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>119</v>
       </c>
@@ -3368,7 +3378,7 @@
       </c>
       <c r="G66" s="22"/>
     </row>
-    <row r="67" spans="1:7" ht="30">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>153</v>
       </c>
@@ -3381,7 +3391,7 @@
       <c r="F67" s="18"/>
       <c r="G67" s="19"/>
     </row>
-    <row r="68" spans="1:7" ht="75">
+    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>121</v>
       </c>
@@ -3398,7 +3408,7 @@
       </c>
       <c r="G68" s="22"/>
     </row>
-    <row r="69" spans="1:7" ht="135">
+    <row r="69" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>122</v>
       </c>
@@ -3415,7 +3425,7 @@
       </c>
       <c r="G69" s="22"/>
     </row>
-    <row r="70" spans="1:7" ht="120">
+    <row r="70" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>123</v>
       </c>
@@ -3432,7 +3442,7 @@
       </c>
       <c r="G70" s="22"/>
     </row>
-    <row r="71" spans="1:7" ht="225">
+    <row r="71" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>124</v>
       </c>
@@ -3449,7 +3459,7 @@
       </c>
       <c r="G71" s="22"/>
     </row>
-    <row r="72" spans="1:7" ht="90">
+    <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>125</v>
       </c>
@@ -3466,7 +3476,7 @@
       </c>
       <c r="G72" s="22"/>
     </row>
-    <row r="73" spans="1:7" ht="165">
+    <row r="73" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>126</v>
       </c>
@@ -3483,7 +3493,7 @@
       </c>
       <c r="G73" s="22"/>
     </row>
-    <row r="74" spans="1:7" ht="30">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
         <v>154</v>
       </c>
@@ -3496,7 +3506,7 @@
       <c r="F74" s="18"/>
       <c r="G74" s="19"/>
     </row>
-    <row r="75" spans="1:7" ht="60">
+    <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>127</v>
       </c>
@@ -3513,7 +3523,7 @@
       </c>
       <c r="G75" s="22"/>
     </row>
-    <row r="76" spans="1:7" ht="150">
+    <row r="76" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>128</v>
       </c>
@@ -3530,7 +3540,7 @@
       </c>
       <c r="G76" s="22"/>
     </row>
-    <row r="77" spans="1:7" ht="60">
+    <row r="77" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>129</v>
       </c>
@@ -3547,7 +3557,7 @@
       </c>
       <c r="G77" s="22"/>
     </row>
-    <row r="78" spans="1:7" ht="45">
+    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
         <v>155</v>
       </c>
@@ -3560,7 +3570,7 @@
       <c r="F78" s="18"/>
       <c r="G78" s="19"/>
     </row>
-    <row r="79" spans="1:7" ht="120">
+    <row r="79" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="23" t="s">
         <v>135</v>
       </c>
@@ -3577,7 +3587,7 @@
       </c>
       <c r="G79" s="22"/>
     </row>
-    <row r="80" spans="1:7" ht="165">
+    <row r="80" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A80" s="23" t="s">
         <v>136</v>
       </c>
@@ -3594,7 +3604,7 @@
       </c>
       <c r="G80" s="22"/>
     </row>
-    <row r="81" spans="1:7" ht="180">
+    <row r="81" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A81" s="23" t="s">
         <v>137</v>
       </c>
@@ -3611,7 +3621,7 @@
       </c>
       <c r="G81" s="22"/>
     </row>
-    <row r="82" spans="1:7" ht="165">
+    <row r="82" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A82" s="23" t="s">
         <v>138</v>
       </c>
@@ -3628,7 +3638,7 @@
       </c>
       <c r="G82" s="22"/>
     </row>
-    <row r="83" spans="1:7" ht="60">
+    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="23" t="s">
         <v>139</v>
       </c>
@@ -3645,7 +3655,7 @@
       </c>
       <c r="G83" s="22"/>
     </row>
-    <row r="84" spans="1:7" ht="165">
+    <row r="84" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" s="23" t="s">
         <v>140</v>
       </c>
@@ -3662,7 +3672,7 @@
       </c>
       <c r="G84" s="22"/>
     </row>
-    <row r="85" spans="1:7" ht="135">
+    <row r="85" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" s="23" t="s">
         <v>141</v>
       </c>
@@ -3679,7 +3689,7 @@
       </c>
       <c r="G85" s="22"/>
     </row>
-    <row r="86" spans="1:7" ht="135">
+    <row r="86" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A86" s="23" t="s">
         <v>142</v>
       </c>
@@ -3696,7 +3706,7 @@
       </c>
       <c r="G86" s="22"/>
     </row>
-    <row r="87" spans="1:7" ht="150">
+    <row r="87" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" s="23" t="s">
         <v>143</v>
       </c>
@@ -3713,7 +3723,7 @@
       </c>
       <c r="G87" s="22"/>
     </row>
-    <row r="88" spans="1:7" ht="165">
+    <row r="88" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A88" s="23" t="s">
         <v>144</v>
       </c>
@@ -3730,7 +3740,7 @@
       </c>
       <c r="G88" s="22"/>
     </row>
-    <row r="89" spans="1:7" ht="135">
+    <row r="89" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A89" s="23" t="s">
         <v>145</v>
       </c>
@@ -3747,7 +3757,7 @@
       </c>
       <c r="G89" s="22"/>
     </row>
-    <row r="90" spans="1:7" ht="165">
+    <row r="90" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A90" s="23" t="s">
         <v>146</v>
       </c>
@@ -3764,7 +3774,7 @@
       </c>
       <c r="G90" s="22"/>
     </row>
-    <row r="91" spans="1:7" ht="135">
+    <row r="91" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A91" s="23" t="s">
         <v>147</v>
       </c>
@@ -3781,7 +3791,7 @@
       </c>
       <c r="G91" s="22"/>
     </row>
-    <row r="92" spans="1:7" ht="150">
+    <row r="92" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A92" s="23" t="s">
         <v>148</v>
       </c>
@@ -3798,7 +3808,7 @@
       </c>
       <c r="G92" s="22"/>
     </row>
-    <row r="93" spans="1:7" ht="45">
+    <row r="93" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
         <v>156</v>
       </c>
@@ -3811,7 +3821,7 @@
       <c r="F93" s="18"/>
       <c r="G93" s="19"/>
     </row>
-    <row r="94" spans="1:7" ht="210">
+    <row r="94" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A94" s="23" t="s">
         <v>149</v>
       </c>
@@ -3828,7 +3838,7 @@
       </c>
       <c r="G94" s="22"/>
     </row>
-    <row r="95" spans="1:7" ht="90">
+    <row r="95" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
         <v>150</v>
       </c>
@@ -3845,7 +3855,7 @@
       </c>
       <c r="G95" s="22"/>
     </row>
-    <row r="96" spans="1:7" ht="195">
+    <row r="96" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A96" s="23" t="s">
         <v>151</v>
       </c>
@@ -3862,7 +3872,7 @@
       </c>
       <c r="G96" s="22"/>
     </row>
-    <row r="97" spans="1:7" ht="30">
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="23" t="s">
         <v>200</v>
       </c>
@@ -3879,7 +3889,7 @@
       </c>
       <c r="G97" s="22"/>
     </row>
-    <row r="98" spans="1:7" ht="60.75" thickBot="1">
+    <row r="98" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="38" t="s">
         <v>201</v>
       </c>
@@ -3896,22 +3906,22 @@
       </c>
       <c r="G98" s="27"/>
     </row>
-    <row r="316" spans="1:1">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="319" spans="1:1">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>8</v>
       </c>
@@ -3954,39 +3964,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -4003,7 +4013,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="44">
         <v>2</v>
       </c>
@@ -4024,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>2.1</v>
       </c>
@@ -4045,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>2.2000000000000002</v>
       </c>
@@ -4066,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="44">
         <v>2.2999999999999998</v>
       </c>
@@ -4087,150 +4097,171 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="44">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="45">
+        <f>COUNTIF(Sheet1!F45:F52, "PASS")</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="45">
+        <f>COUNTIF(Sheet1!F45:F52, "FAIL")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="45">
+        <f>COUNTIF(Sheet1!F45:F52, "NOT RUN")</f>
+        <v>8</v>
+      </c>
+      <c r="E11" s="45">
+        <f>COUNTIF(Sheet1!F45:F52, BLOCKED)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
         <v>2.4</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B12" s="45">
         <f>COUNTIF(Sheet1!F54:F60, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C12" s="45">
         <f>COUNTIF(Sheet1!F54:F60, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D11" s="45">
+      <c r="D12" s="45">
         <f>COUNTIF(Sheet1!F54:F60, "NOT RUN")</f>
         <v>7</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E12" s="45">
         <f>COUNTIF(Sheet1!F54:F60, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="44">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="44">
         <v>2.5</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B13" s="45">
         <f>COUNTIF(Sheet1!F62:F66, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C13" s="45">
         <f>COUNTIF(Sheet1!F62:F66, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D12" s="45">
+      <c r="D13" s="45">
         <f>COUNTIF(Sheet1!F62:F66, "NOT RUN")</f>
         <v>5</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E13" s="45">
         <f>COUNTIF(Sheet1!F62:F66, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="44" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="B13" s="45">
+      <c r="B14" s="45">
         <f>COUNTIF(Sheet1!F68:F73, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C14" s="45">
         <f>COUNTIF(Sheet1!F68:F73, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D13" s="45">
+      <c r="D14" s="45">
         <f>COUNTIF(Sheet1!F68:F73, "NOT RUN")</f>
         <v>6</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E14" s="45">
         <f>COUNTIF(Sheet1!F68:F73, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="44" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="45">
+      <c r="B15" s="45">
         <f>COUNTIF(Sheet1!F75:F77, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C14" s="45">
+      <c r="C15" s="45">
         <f>COUNTIF(Sheet1!F75:F77, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D15" s="45">
         <f>COUNTIF(Sheet1!F75:F77, "NOT RUN")</f>
         <v>3</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E15" s="45">
         <f>COUNTIF(Sheet1!F75:F77, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="44" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="45">
+      <c r="B16" s="45">
         <f>COUNTIF(Sheet1!F79:F92, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C15" s="45">
+      <c r="C16" s="45">
         <f>COUNTIF(Sheet1!F79:F92, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D15" s="45">
+      <c r="D16" s="45">
         <f>COUNTIF(Sheet1!F79:F92, "NOT RUN")</f>
         <v>14</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E16" s="45">
         <f>COUNTIF(Sheet1!F79:F92, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="44" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="B16" s="45">
+      <c r="B17" s="45">
         <f>COUNTIF(Sheet1!F94:F98, "PASS")</f>
         <v>0</v>
       </c>
-      <c r="C16" s="45">
+      <c r="C17" s="45">
         <f>COUNTIF(Sheet1!F94:F98, "FAIL")</f>
         <v>0</v>
       </c>
-      <c r="D16" s="45">
+      <c r="D17" s="45">
         <f>COUNTIF(Sheet1!F94:F98, "NOT RUN")</f>
         <v>5</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E17" s="45">
         <f>COUNTIF(Sheet1!F94:F98, "BLOCKED")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="44" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="B17">
-        <f>SUM(B7:B16)</f>
+      <c r="B18">
+        <f>SUM(B7:B17)</f>
         <v>0</v>
       </c>
-      <c r="C17">
-        <f>SUM(C7:C16)</f>
+      <c r="C18">
+        <f>SUM(C7:C17)</f>
         <v>0</v>
       </c>
-      <c r="D17">
-        <f>SUM(D7:D16)</f>
-        <v>74</v>
-      </c>
-      <c r="E17">
-        <f>SUM(E7:E16)</f>
+      <c r="D18">
+        <f>SUM(D7:D17)</f>
+        <v>82</v>
+      </c>
+      <c r="E18">
+        <f>SUM(E7:E17)</f>
         <v>0</v>
       </c>
     </row>
@@ -4240,31 +4271,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>

</xml_diff>